<commit_message>
Antimicrobial extract EthOH new analysis.
</commit_message>
<xml_diff>
--- a/Data/Antimicrobial_H2O_EthOH_Chakra_B.xlsx
+++ b/Data/Antimicrobial_H2O_EthOH_Chakra_B.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F4ss0\Documents\Ikiam21062022\Proyecto Guayusa\Antimicrobial_I_guayusa\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2DBBCE-6393-4EAC-B307-458A99903D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E926946B-8A3B-4841-971F-BD1D1B818F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="5" xr2:uid="{AE241DF6-4FFC-4DF2-B60A-123CF49BB9C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{AE241DF6-4FFC-4DF2-B60A-123CF49BB9C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Escalas" sheetId="1" r:id="rId1"/>
@@ -1931,7 +1931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8542F08-6268-4576-8880-7C096C0A263D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1982,7 +1982,8 @@
         <v>6.228369542958232</v>
       </c>
       <c r="B4">
-        <v>27.969000000000001</v>
+        <f>AVERAGE(B2:B3)</f>
+        <v>32.7515</v>
       </c>
       <c r="C4">
         <v>10.585076955155774</v>
@@ -2138,7 +2139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60593CFE-100E-485A-AB91-C94FDA48628B}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>